<commit_message>
Initial DBF to CVS export
</commit_message>
<xml_diff>
--- a/metadata/metasheet.xlsx
+++ b/metadata/metasheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pascal/Work/Python/metasheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/WDPassport/DataArchive/NIJ/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5780" yWindow="1040" windowWidth="29920" windowHeight="18720" tabRatio="500"/>
+    <workbookView xWindow="5380" yWindow="1920" windowWidth="29920" windowHeight="18720" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="variables" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="39">
   <si>
     <t>bank</t>
   </si>
@@ -105,6 +105,51 @@
   </si>
   <si>
     <t>onFail</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>call_group</t>
+  </si>
+  <si>
+    <t>final_case</t>
+  </si>
+  <si>
+    <t>case_desc</t>
+  </si>
+  <si>
+    <t>occ_date</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t>NIJ_CFS_RL</t>
+  </si>
+  <si>
+    <t>NIJ_CFS_VARS</t>
+  </si>
+  <si>
+    <t>cfs_dbf</t>
+  </si>
+  <si>
+    <t>calls-for-service DBF</t>
+  </si>
+  <si>
+    <t>date(iso8601)</t>
+  </si>
+  <si>
+    <t>x_coordina</t>
+  </si>
+  <si>
+    <t>y_coordina</t>
+  </si>
+  <si>
+    <t>census_tra</t>
   </si>
 </sst>
 </file>
@@ -473,19 +518,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="1"/>
-    <col min="3" max="3" width="12.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="40.1640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="10.83203125" style="1"/>
@@ -518,36 +563,106 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E2" s="1"/>
+      <c r="A2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E10" s="1"/>
@@ -823,11 +938,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:F1"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -858,6 +973,20 @@
         <v>16</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -865,11 +994,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -898,6 +1027,70 @@
       </c>
       <c r="F1" s="3" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Package data and metadata
</commit_message>
<xml_diff>
--- a/metadata/metasheet.xlsx
+++ b/metadata/metasheet.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/WDPassport/DataArchive/NIJ/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pascal/DataArchive/us-nij-rtcfc/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5300" yWindow="1280" windowWidth="29920" windowHeight="18720" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="3520" yWindow="1260" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="variables" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="157">
   <si>
     <t>bank</t>
   </si>
@@ -164,9 +164,6 @@
     <t>PERSON CRIME</t>
   </si>
   <si>
-    <t xml:space="preserve"> SUSPICIOUS</t>
-  </si>
-  <si>
     <t>NON CRIMINAL/ADMIN</t>
   </si>
   <si>
@@ -176,246 +173,78 @@
     <t>TRAFFIC</t>
   </si>
   <si>
-    <t xml:space="preserve">DISTP </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DISTW </t>
-  </si>
-  <si>
-    <t xml:space="preserve">VICE  </t>
-  </si>
-  <si>
     <t>ASSLTP</t>
   </si>
   <si>
     <t>ASSLTW</t>
   </si>
   <si>
-    <t xml:space="preserve">ROBP  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROBW  </t>
-  </si>
-  <si>
     <t>SHOOTW</t>
   </si>
   <si>
-    <t xml:space="preserve">SHOTS </t>
-  </si>
-  <si>
-    <t xml:space="preserve">STABW </t>
-  </si>
-  <si>
     <t>THRETP</t>
   </si>
   <si>
     <t>THRETW</t>
   </si>
   <si>
-    <t xml:space="preserve">GANG  </t>
-  </si>
-  <si>
     <t>AREACK</t>
   </si>
   <si>
     <t>PREMCK</t>
   </si>
   <si>
-    <t xml:space="preserve">SUSP  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SUSPP </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SUSPW </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANIML </t>
-  </si>
-  <si>
     <t>ANIMLP</t>
   </si>
   <si>
     <t>BOMBTH</t>
   </si>
   <si>
-    <t xml:space="preserve">DIST  </t>
-  </si>
-  <si>
     <t>ESCAPE</t>
   </si>
   <si>
-    <t xml:space="preserve">FWB   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FWH   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FWI   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHEM  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FWN   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOISE </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PARK  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PARTY </t>
-  </si>
-  <si>
     <t>POLINV</t>
   </si>
   <si>
-    <t xml:space="preserve">SCHL  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCHLP </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCHLW </t>
-  </si>
-  <si>
-    <t xml:space="preserve">THRET </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TMET  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TMETP </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TMETW </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRASH </t>
-  </si>
-  <si>
     <t>TRASHP</t>
   </si>
   <si>
-    <t xml:space="preserve">UNWNT </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FPURS </t>
-  </si>
-  <si>
     <t>UNWNTW</t>
   </si>
   <si>
-    <t xml:space="preserve">W26   </t>
-  </si>
-  <si>
     <t>ASSIST</t>
   </si>
   <si>
-    <t xml:space="preserve">CIVIL </t>
-  </si>
-  <si>
-    <t xml:space="preserve">EVICT </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FLAG  </t>
-  </si>
-  <si>
     <t>FOLLOW</t>
   </si>
   <si>
-    <t xml:space="preserve">MSG   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PROP  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GREAT </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RED   </t>
-  </si>
-  <si>
     <t>RIVPOL</t>
   </si>
   <si>
     <t>SCHLET</t>
   </si>
   <si>
-    <t xml:space="preserve">SERVE </t>
-  </si>
-  <si>
     <t>STNDBY</t>
   </si>
   <si>
     <t>SUBSTP</t>
   </si>
   <si>
-    <t xml:space="preserve">TRANS </t>
-  </si>
-  <si>
-    <t xml:space="preserve">WARR  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">WELCK </t>
-  </si>
-  <si>
-    <t xml:space="preserve">WARRC </t>
-  </si>
-  <si>
     <t>WELCKP</t>
   </si>
   <si>
-    <t xml:space="preserve">ASSLT </t>
-  </si>
-  <si>
     <t>DEVICE</t>
   </si>
   <si>
-    <t xml:space="preserve">ROB   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHOOT </t>
-  </si>
-  <si>
-    <t xml:space="preserve">STAB  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BURG  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FRAUD </t>
-  </si>
-  <si>
     <t>FRAUDP</t>
   </si>
   <si>
-    <t xml:space="preserve">THEFT </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IDENT </t>
-  </si>
-  <si>
     <t>THEFTC</t>
   </si>
   <si>
     <t>THEFTP</t>
   </si>
   <si>
-    <t xml:space="preserve">VAND  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">VANDP </t>
-  </si>
-  <si>
-    <t xml:space="preserve">VEHST </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACCHR </t>
-  </si>
-  <si>
     <t>ACCHRP</t>
   </si>
   <si>
@@ -431,24 +260,12 @@
     <t>ACCUNK</t>
   </si>
   <si>
-    <t xml:space="preserve">DUII  </t>
-  </si>
-  <si>
     <t>HAZARD</t>
   </si>
   <si>
     <t>TRASTP</t>
   </si>
   <si>
-    <t xml:space="preserve">WRONG </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TPURS </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RSTLN </t>
-  </si>
-  <si>
     <t>VEHREC</t>
   </si>
   <si>
@@ -458,9 +275,6 @@
     <t>PROWLP</t>
   </si>
   <si>
-    <t xml:space="preserve">BURGP </t>
-  </si>
-  <si>
     <t>77</t>
   </si>
   <si>
@@ -479,10 +293,217 @@
     <t>BUR</t>
   </si>
   <si>
-    <t>call_groups</t>
-  </si>
-  <si>
     <t>case_type</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Call group</t>
+  </si>
+  <si>
+    <t>Final case type</t>
+  </si>
+  <si>
+    <t>Case description</t>
+  </si>
+  <si>
+    <t>Occurrence date</t>
+  </si>
+  <si>
+    <t>Y coordinate</t>
+  </si>
+  <si>
+    <t>Census tract</t>
+  </si>
+  <si>
+    <t>X coordinate</t>
+  </si>
+  <si>
+    <t>DISTP</t>
+  </si>
+  <si>
+    <t>DISTW</t>
+  </si>
+  <si>
+    <t>VICE</t>
+  </si>
+  <si>
+    <t>ROBP</t>
+  </si>
+  <si>
+    <t>ROBW</t>
+  </si>
+  <si>
+    <t>SHOTS</t>
+  </si>
+  <si>
+    <t>STABW</t>
+  </si>
+  <si>
+    <t>GANG</t>
+  </si>
+  <si>
+    <t>SUSP</t>
+  </si>
+  <si>
+    <t>SUSPP</t>
+  </si>
+  <si>
+    <t>SUSPW</t>
+  </si>
+  <si>
+    <t>ANIML</t>
+  </si>
+  <si>
+    <t>DIST</t>
+  </si>
+  <si>
+    <t>FWB</t>
+  </si>
+  <si>
+    <t>FWH</t>
+  </si>
+  <si>
+    <t>FWI</t>
+  </si>
+  <si>
+    <t>CHEM</t>
+  </si>
+  <si>
+    <t>FWN</t>
+  </si>
+  <si>
+    <t>NOISE</t>
+  </si>
+  <si>
+    <t>PARK</t>
+  </si>
+  <si>
+    <t>PARTY</t>
+  </si>
+  <si>
+    <t>SCHL</t>
+  </si>
+  <si>
+    <t>SCHLP</t>
+  </si>
+  <si>
+    <t>SCHLW</t>
+  </si>
+  <si>
+    <t>THRET</t>
+  </si>
+  <si>
+    <t>TMET</t>
+  </si>
+  <si>
+    <t>TMETP</t>
+  </si>
+  <si>
+    <t>TMETW</t>
+  </si>
+  <si>
+    <t>TRASH</t>
+  </si>
+  <si>
+    <t>UNWNT</t>
+  </si>
+  <si>
+    <t>FPURS</t>
+  </si>
+  <si>
+    <t>W26</t>
+  </si>
+  <si>
+    <t>CIVIL</t>
+  </si>
+  <si>
+    <t>EVICT</t>
+  </si>
+  <si>
+    <t>FLAG</t>
+  </si>
+  <si>
+    <t>MSG</t>
+  </si>
+  <si>
+    <t>PROP</t>
+  </si>
+  <si>
+    <t>GREAT</t>
+  </si>
+  <si>
+    <t>RED</t>
+  </si>
+  <si>
+    <t>SERVE</t>
+  </si>
+  <si>
+    <t>TRANS</t>
+  </si>
+  <si>
+    <t>WARR</t>
+  </si>
+  <si>
+    <t>WELCK</t>
+  </si>
+  <si>
+    <t>WARRC</t>
+  </si>
+  <si>
+    <t>ASSLT</t>
+  </si>
+  <si>
+    <t>ROB</t>
+  </si>
+  <si>
+    <t>SHOOT</t>
+  </si>
+  <si>
+    <t>STAB</t>
+  </si>
+  <si>
+    <t>BURG</t>
+  </si>
+  <si>
+    <t>FRAUD</t>
+  </si>
+  <si>
+    <t>THEFT</t>
+  </si>
+  <si>
+    <t>IDENT</t>
+  </si>
+  <si>
+    <t>VAND</t>
+  </si>
+  <si>
+    <t>VANDP</t>
+  </si>
+  <si>
+    <t>VEHST</t>
+  </si>
+  <si>
+    <t>ACCHR</t>
+  </si>
+  <si>
+    <t>DUII</t>
+  </si>
+  <si>
+    <t>WRONG</t>
+  </si>
+  <si>
+    <t>TPURS</t>
+  </si>
+  <si>
+    <t>RSTLN</t>
+  </si>
+  <si>
+    <t>BURGP</t>
+  </si>
+  <si>
+    <t>SUSPICIOUS</t>
   </si>
 </sst>
 </file>
@@ -854,7 +875,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -903,12 +924,18 @@
       <c r="C2" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="E2" s="1" t="s">
         <v>26</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1">
-        <v>254</v>
+        <v>3</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -918,12 +945,18 @@
       <c r="C3" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="D3" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="E3" s="1" t="s">
         <v>26</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1">
-        <v>254</v>
+        <v>20</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -933,12 +966,18 @@
       <c r="C4" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="E4" s="1" t="s">
         <v>26</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1">
-        <v>254</v>
+        <v>6</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -948,12 +987,15 @@
       <c r="C5" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="D5" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="E5" s="1" t="s">
         <v>26</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1">
-        <v>254</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -963,6 +1005,9 @@
       <c r="C6" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="D6" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E6" s="1" t="s">
         <v>32</v>
       </c>
@@ -978,6 +1023,9 @@
       <c r="C7" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="D7" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="E7" s="1" t="s">
         <v>27</v>
       </c>
@@ -985,7 +1033,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="1">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -995,6 +1043,9 @@
       <c r="C8" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="D8" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="E8" s="1" t="s">
         <v>27</v>
       </c>
@@ -1002,7 +1053,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="1">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -1012,14 +1063,17 @@
       <c r="C9" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="D9" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="E9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F9" s="1">
         <v>0</v>
       </c>
       <c r="G9" s="1">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -1236,7 +1290,7 @@
       <pane xSplit="9" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1259,7 +1313,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>143</v>
+        <v>81</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>22</v>
@@ -1267,18 +1321,18 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>143</v>
+        <v>81</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>148</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>143</v>
+        <v>81</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1291,8 +1345,8 @@
   <dimension ref="A1:C109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1319,7 +1373,7 @@
         <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>146</v>
+        <v>84</v>
       </c>
       <c r="C2" t="s">
         <v>37</v>
@@ -1330,7 +1384,7 @@
         <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>144</v>
+        <v>82</v>
       </c>
       <c r="C3" t="s">
         <v>38</v>
@@ -1341,7 +1395,7 @@
         <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>145</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
         <v>39</v>
@@ -1352,7 +1406,7 @@
         <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>147</v>
+        <v>85</v>
       </c>
       <c r="C5" t="s">
         <v>40</v>
@@ -1360,7 +1414,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>148</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
         <v>41</v>
@@ -1371,7 +1425,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>148</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
         <v>42</v>
@@ -1382,1102 +1436,1102 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>148</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>156</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>148</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>148</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>148</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>95</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>96</v>
       </c>
       <c r="C15" t="s">
-        <v>48</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>97</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>98</v>
       </c>
       <c r="C19" t="s">
-        <v>52</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B20" t="s">
-        <v>53</v>
+        <v>99</v>
       </c>
       <c r="C20" t="s">
-        <v>53</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B21" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C21" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>100</v>
       </c>
       <c r="C22" t="s">
-        <v>55</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B23" t="s">
-        <v>56</v>
+        <v>101</v>
       </c>
       <c r="C23" t="s">
-        <v>56</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B24" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C24" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B25" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C25" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B26" t="s">
-        <v>59</v>
+        <v>102</v>
       </c>
       <c r="C26" t="s">
-        <v>59</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B27" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C27" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B28" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C28" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B29" t="s">
-        <v>62</v>
+        <v>103</v>
       </c>
       <c r="C29" t="s">
-        <v>62</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B30" t="s">
-        <v>63</v>
+        <v>104</v>
       </c>
       <c r="C30" t="s">
-        <v>63</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B31" t="s">
-        <v>64</v>
+        <v>105</v>
       </c>
       <c r="C31" t="s">
-        <v>64</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B32" t="s">
-        <v>65</v>
+        <v>106</v>
       </c>
       <c r="C32" t="s">
-        <v>65</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B33" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C33" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B34" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="C34" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B35" t="s">
-        <v>68</v>
+        <v>107</v>
       </c>
       <c r="C35" t="s">
-        <v>68</v>
+        <v>107</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B36" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="C36" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B37" t="s">
-        <v>70</v>
+        <v>108</v>
       </c>
       <c r="C37" t="s">
-        <v>70</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B38" t="s">
-        <v>71</v>
+        <v>109</v>
       </c>
       <c r="C38" t="s">
-        <v>71</v>
+        <v>109</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B39" t="s">
-        <v>72</v>
+        <v>110</v>
       </c>
       <c r="C39" t="s">
-        <v>72</v>
+        <v>110</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B40" t="s">
-        <v>73</v>
+        <v>111</v>
       </c>
       <c r="C40" t="s">
-        <v>73</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B41" t="s">
-        <v>74</v>
+        <v>112</v>
       </c>
       <c r="C41" t="s">
-        <v>74</v>
+        <v>112</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B42" t="s">
-        <v>75</v>
+        <v>113</v>
       </c>
       <c r="C42" t="s">
-        <v>75</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B43" t="s">
-        <v>76</v>
+        <v>114</v>
       </c>
       <c r="C43" t="s">
-        <v>76</v>
+        <v>114</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B44" t="s">
-        <v>77</v>
+        <v>115</v>
       </c>
       <c r="C44" t="s">
-        <v>77</v>
+        <v>115</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B45" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="C45" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B46" t="s">
-        <v>79</v>
+        <v>116</v>
       </c>
       <c r="C46" t="s">
-        <v>79</v>
+        <v>116</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B47" t="s">
-        <v>80</v>
+        <v>117</v>
       </c>
       <c r="C47" t="s">
-        <v>80</v>
+        <v>117</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B48" t="s">
-        <v>81</v>
+        <v>118</v>
       </c>
       <c r="C48" t="s">
-        <v>81</v>
+        <v>118</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B49" t="s">
-        <v>82</v>
+        <v>119</v>
       </c>
       <c r="C49" t="s">
-        <v>82</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B50" t="s">
-        <v>83</v>
+        <v>120</v>
       </c>
       <c r="C50" t="s">
-        <v>83</v>
+        <v>120</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B51" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
       <c r="C51" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B52" t="s">
-        <v>85</v>
+        <v>122</v>
       </c>
       <c r="C52" t="s">
-        <v>85</v>
+        <v>122</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B53" t="s">
-        <v>86</v>
+        <v>123</v>
       </c>
       <c r="C53" t="s">
-        <v>86</v>
+        <v>123</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B54" t="s">
-        <v>87</v>
+        <v>57</v>
       </c>
       <c r="C54" t="s">
-        <v>87</v>
+        <v>57</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B55" t="s">
-        <v>88</v>
+        <v>124</v>
       </c>
       <c r="C55" t="s">
-        <v>88</v>
+        <v>124</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B56" t="s">
-        <v>89</v>
+        <v>125</v>
       </c>
       <c r="C56" t="s">
-        <v>89</v>
+        <v>125</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B57" t="s">
-        <v>90</v>
+        <v>58</v>
       </c>
       <c r="C57" t="s">
-        <v>90</v>
+        <v>58</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B58" t="s">
-        <v>91</v>
+        <v>126</v>
       </c>
       <c r="C58" t="s">
-        <v>91</v>
+        <v>126</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>142</v>
+        <v>80</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>142</v>
+        <v>80</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B60" t="s">
-        <v>92</v>
+        <v>59</v>
       </c>
       <c r="C60" t="s">
-        <v>92</v>
+        <v>59</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B61" t="s">
-        <v>93</v>
+        <v>127</v>
       </c>
       <c r="C61" t="s">
-        <v>93</v>
+        <v>127</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B62" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="C62" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B63" t="s">
-        <v>95</v>
+        <v>129</v>
       </c>
       <c r="C63" t="s">
-        <v>95</v>
+        <v>129</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B64" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
       <c r="C64" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B65" t="s">
-        <v>97</v>
+        <v>130</v>
       </c>
       <c r="C65" t="s">
-        <v>97</v>
+        <v>130</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B66" t="s">
-        <v>98</v>
+        <v>131</v>
       </c>
       <c r="C66" t="s">
-        <v>98</v>
+        <v>131</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B67" t="s">
-        <v>99</v>
+        <v>132</v>
       </c>
       <c r="C67" t="s">
-        <v>99</v>
+        <v>132</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B68" t="s">
-        <v>100</v>
+        <v>133</v>
       </c>
       <c r="C68" t="s">
-        <v>100</v>
+        <v>133</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B69" t="s">
-        <v>101</v>
+        <v>61</v>
       </c>
       <c r="C69" t="s">
-        <v>101</v>
+        <v>61</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B70" t="s">
-        <v>102</v>
+        <v>62</v>
       </c>
       <c r="C70" t="s">
-        <v>102</v>
+        <v>62</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B71" t="s">
-        <v>103</v>
+        <v>134</v>
       </c>
       <c r="C71" t="s">
-        <v>103</v>
+        <v>134</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B72" t="s">
-        <v>104</v>
+        <v>63</v>
       </c>
       <c r="C72" t="s">
-        <v>104</v>
+        <v>63</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B73" t="s">
-        <v>105</v>
+        <v>64</v>
       </c>
       <c r="C73" t="s">
-        <v>105</v>
+        <v>64</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B74" t="s">
-        <v>106</v>
+        <v>135</v>
       </c>
       <c r="C74" t="s">
-        <v>106</v>
+        <v>135</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B75" t="s">
-        <v>107</v>
+        <v>136</v>
       </c>
       <c r="C75" t="s">
-        <v>107</v>
+        <v>136</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B76" t="s">
-        <v>108</v>
+        <v>137</v>
       </c>
       <c r="C76" t="s">
-        <v>108</v>
+        <v>137</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B77" t="s">
-        <v>109</v>
+        <v>138</v>
       </c>
       <c r="C77" t="s">
-        <v>109</v>
+        <v>138</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B78" t="s">
-        <v>110</v>
+        <v>65</v>
       </c>
       <c r="C78" t="s">
-        <v>110</v>
+        <v>65</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B79" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="C79" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B80" t="s">
-        <v>112</v>
+        <v>66</v>
       </c>
       <c r="C80" t="s">
-        <v>112</v>
+        <v>66</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B81" t="s">
-        <v>113</v>
+        <v>140</v>
       </c>
       <c r="C81" t="s">
-        <v>113</v>
+        <v>140</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B82" t="s">
-        <v>114</v>
+        <v>141</v>
       </c>
       <c r="C82" t="s">
-        <v>114</v>
+        <v>141</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B83" t="s">
-        <v>115</v>
+        <v>142</v>
       </c>
       <c r="C83" t="s">
-        <v>115</v>
+        <v>142</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B84" t="s">
-        <v>116</v>
+        <v>143</v>
       </c>
       <c r="C84" t="s">
-        <v>116</v>
+        <v>143</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B85" t="s">
-        <v>117</v>
+        <v>144</v>
       </c>
       <c r="C85" t="s">
-        <v>117</v>
+        <v>144</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B86" t="s">
-        <v>118</v>
+        <v>67</v>
       </c>
       <c r="C86" t="s">
-        <v>118</v>
+        <v>67</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>119</v>
+        <v>145</v>
       </c>
       <c r="C87" t="s">
-        <v>119</v>
+        <v>145</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>120</v>
+        <v>146</v>
       </c>
       <c r="C88" t="s">
-        <v>120</v>
+        <v>146</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B89" t="s">
-        <v>121</v>
+        <v>68</v>
       </c>
       <c r="C89" t="s">
-        <v>121</v>
+        <v>68</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B90" t="s">
-        <v>122</v>
+        <v>69</v>
       </c>
       <c r="C90" t="s">
-        <v>122</v>
+        <v>69</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B91" t="s">
-        <v>123</v>
+        <v>147</v>
       </c>
       <c r="C91" t="s">
-        <v>123</v>
+        <v>147</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B92" t="s">
-        <v>124</v>
+        <v>148</v>
       </c>
       <c r="C92" t="s">
-        <v>124</v>
+        <v>148</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B93" t="s">
         <v>149</v>
       </c>
-      <c r="B93" t="s">
-        <v>125</v>
-      </c>
       <c r="C93" t="s">
-        <v>125</v>
+        <v>149</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B94" t="s">
-        <v>126</v>
+        <v>150</v>
       </c>
       <c r="C94" t="s">
-        <v>126</v>
+        <v>150</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B95" t="s">
-        <v>127</v>
+        <v>70</v>
       </c>
       <c r="C95" t="s">
-        <v>127</v>
+        <v>70</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B96" t="s">
-        <v>128</v>
+        <v>71</v>
       </c>
       <c r="C96" t="s">
-        <v>128</v>
+        <v>71</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B97" t="s">
-        <v>129</v>
+        <v>72</v>
       </c>
       <c r="C97" t="s">
-        <v>129</v>
+        <v>72</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B98" t="s">
-        <v>130</v>
+        <v>73</v>
       </c>
       <c r="C98" t="s">
-        <v>130</v>
+        <v>73</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B99" t="s">
-        <v>131</v>
+        <v>74</v>
       </c>
       <c r="C99" t="s">
-        <v>131</v>
+        <v>74</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B100" t="s">
-        <v>132</v>
+        <v>151</v>
       </c>
       <c r="C100" t="s">
-        <v>132</v>
+        <v>151</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B101" t="s">
-        <v>133</v>
+        <v>75</v>
       </c>
       <c r="C101" t="s">
-        <v>133</v>
+        <v>75</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B102" t="s">
-        <v>134</v>
+        <v>76</v>
       </c>
       <c r="C102" t="s">
-        <v>134</v>
+        <v>76</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B103" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
       <c r="C103" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B104" t="s">
-        <v>136</v>
+        <v>153</v>
       </c>
       <c r="C104" t="s">
-        <v>136</v>
+        <v>153</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B105" t="s">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="C105" t="s">
-        <v>137</v>
+        <v>154</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B106" t="s">
-        <v>138</v>
+        <v>77</v>
       </c>
       <c r="C106" t="s">
-        <v>138</v>
+        <v>77</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B107" t="s">
-        <v>139</v>
+        <v>78</v>
       </c>
       <c r="C107" t="s">
-        <v>139</v>
+        <v>78</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B108" t="s">
-        <v>140</v>
+        <v>79</v>
       </c>
       <c r="C108" t="s">
-        <v>140</v>
+        <v>79</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="B109" t="s">
-        <v>141</v>
+        <v>155</v>
       </c>
       <c r="C109" t="s">
-        <v>141</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -2547,7 +2601,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>